<commit_message>
Renamed tabs to reflect their contents.
</commit_message>
<xml_diff>
--- a/CDA-to-FHIR_mappings.xlsx
+++ b/CDA-to-FHIR_mappings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeanduteau/Dropbox (DDI Work)/HL7 CCDA FHIR Mapping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeanduteau/Dropbox (DDI Work)/HL7 CCDA FHIR Mapping/git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78A44C1-C07C-1E48-BBEB-7A20143ACEB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DFC18C-354D-6646-B7D6-D1C31CDE7177}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7160" yWindow="1180" windowWidth="32580" windowHeight="26840" xr2:uid="{BECB9657-49B2-1141-A8A5-81EA227BF036}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="AllergyIntolerance" sheetId="3" r:id="rId3"/>
     <sheet name="Problem" sheetId="10" r:id="rId4"/>
     <sheet name="MedicationActivity" sheetId="5" r:id="rId5"/>
-    <sheet name="Problem Acts" sheetId="12" r:id="rId6"/>
+    <sheet name="Procedure Acts" sheetId="12" r:id="rId6"/>
     <sheet name="Results" sheetId="15" r:id="rId7"/>
     <sheet name="Planned Acts" sheetId="6" r:id="rId8"/>
     <sheet name="Social History" sheetId="18" r:id="rId9"/>

</xml_diff>

<commit_message>
Family History and Nutrition mappings.
</commit_message>
<xml_diff>
--- a/CDA-to-FHIR_mappings.xlsx
+++ b/CDA-to-FHIR_mappings.xlsx
@@ -8,33 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeanduteau/Dropbox (DDI Work)/HL7 CCDA FHIR Mapping/git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DFC18C-354D-6646-B7D6-D1C31CDE7177}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FD2742-3314-104F-85FF-A2E5581956BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7160" yWindow="1180" windowWidth="32580" windowHeight="26840" xr2:uid="{BECB9657-49B2-1141-A8A5-81EA227BF036}"/>
+    <workbookView xWindow="18560" yWindow="740" windowWidth="32580" windowHeight="26840" xr2:uid="{BECB9657-49B2-1141-A8A5-81EA227BF036}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="17" r:id="rId1"/>
     <sheet name="ClinicalDocument" sheetId="1" r:id="rId2"/>
     <sheet name="AllergyIntolerance" sheetId="3" r:id="rId3"/>
-    <sheet name="Problem" sheetId="10" r:id="rId4"/>
-    <sheet name="MedicationActivity" sheetId="5" r:id="rId5"/>
-    <sheet name="Procedure Acts" sheetId="12" r:id="rId6"/>
-    <sheet name="Results" sheetId="15" r:id="rId7"/>
-    <sheet name="Planned Acts" sheetId="6" r:id="rId8"/>
-    <sheet name="Social History" sheetId="18" r:id="rId9"/>
-    <sheet name="Assorted" sheetId="2" r:id="rId10"/>
+    <sheet name="FamilyHistory" sheetId="19" r:id="rId4"/>
+    <sheet name="Nutrition" sheetId="20" r:id="rId5"/>
+    <sheet name="Problem" sheetId="10" r:id="rId6"/>
+    <sheet name="MedicationActivity" sheetId="5" r:id="rId7"/>
+    <sheet name="Procedure Acts" sheetId="12" r:id="rId8"/>
+    <sheet name="Results" sheetId="15" r:id="rId9"/>
+    <sheet name="Planned Acts" sheetId="6" r:id="rId10"/>
+    <sheet name="Social History" sheetId="18" r:id="rId11"/>
+    <sheet name="Assorted" sheetId="2" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="457">
   <si>
     <t>realmCode</t>
   </si>
@@ -1107,9 +1114,6 @@
     <t>Problem Observation</t>
   </si>
   <si>
-    <t>included by Hospital Discharge Diagnosis</t>
-  </si>
-  <si>
     <t>included by Discharge Medication, includes Medication Information</t>
   </si>
   <si>
@@ -1342,6 +1346,72 @@
   </si>
   <si>
     <t>TOBACCOUSE (observation)</t>
+  </si>
+  <si>
+    <t>FAMILYHISTORYORGANIZER(CLUSTER)</t>
+  </si>
+  <si>
+    <t>relatedSubject</t>
+  </si>
+  <si>
+    <t>entryRelationship (FamilyHistoryDeathObservation: observation)</t>
+  </si>
+  <si>
+    <t>FAMILYMEMBERHISTORY</t>
+  </si>
+  <si>
+    <t>FamilyMemberHistory.relationship</t>
+  </si>
+  <si>
+    <t>FamilyMemberHistory.identifier</t>
+  </si>
+  <si>
+    <t>FamilyMemberHistory.gender</t>
+  </si>
+  <si>
+    <t>FamilyMemberHistory.bornDate</t>
+  </si>
+  <si>
+    <t>FamilyMemberHistory.condition.code</t>
+  </si>
+  <si>
+    <t>FamilyMemberHistory.condition.onsetAge</t>
+  </si>
+  <si>
+    <t>FamilyMemberHistory.deceasedBoolean</t>
+  </si>
+  <si>
+    <t>FamilyMemberHistory.condition</t>
+  </si>
+  <si>
+    <t>Family History Organizer</t>
+  </si>
+  <si>
+    <t>included by Hospital Discharge Diagnosis, includes Prognosis Observation and Age Observation (for Problems)</t>
+  </si>
+  <si>
+    <t>includes Family History Observation and Age Observation (for Family History)</t>
+  </si>
+  <si>
+    <t>NUTRITIONALSTATUSOBSERVATION(OBSERVATION)</t>
+  </si>
+  <si>
+    <t>entryRelationship(NutritionAssessment: observation)</t>
+  </si>
+  <si>
+    <t>Observation.effectiveDateTime</t>
+  </si>
+  <si>
+    <t>NUTRITIONASSESSMENT(OBSERVATION)</t>
+  </si>
+  <si>
+    <t>Nutritional Status Observation</t>
+  </si>
+  <si>
+    <t>Nutrition Assessment</t>
+  </si>
+  <si>
+    <t>includes Estimated Date of Delivery</t>
   </si>
 </sst>
 </file>
@@ -1714,10 +1784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF0DF62-6E02-AB44-80BE-5CCD9B30E57D}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1738,7 +1808,7 @@
         <v>351</v>
       </c>
       <c r="B3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1754,7 +1824,7 @@
         <v>354</v>
       </c>
       <c r="B5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1764,27 +1834,27 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1792,73 +1862,94 @@
         <v>356</v>
       </c>
       <c r="B12" t="s">
-        <v>357</v>
+        <v>448</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
+      </c>
+      <c r="B13" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B16" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="B26" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -1886,12 +1977,693 @@
     <hyperlink ref="A20" location="'Social History'!A19" display="Smoking Status - MeaningfulUse" xr:uid="{3C75D9A5-D3B4-B84E-985F-22243BF0391B}"/>
     <hyperlink ref="A22" location="'Social History'!A28" display="Tobacco Use" xr:uid="{808F0D15-1668-7748-B694-D2FFA3BC3DDF}"/>
     <hyperlink ref="A21" location="'Social History'!A1" display="Social History Observation" xr:uid="{CD526A3C-1E5B-3E44-B965-588E7C095110}"/>
+    <hyperlink ref="A26" location="FamilyHistory!A1" display="Family History Organizer" xr:uid="{CB64A738-46D4-6648-A2A0-41C7A02D4566}"/>
+    <hyperlink ref="A27" location="Nutrition!A1" display="Nutritional Status Observation" xr:uid="{868E2CDE-4EB7-604D-9185-D9167243EC65}"/>
+    <hyperlink ref="A28" location="Nutrition!A8" display="Nutrition Assessment" xr:uid="{DCDCA9D0-860B-1640-91B4-DAF0FCF300E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E45DC903-E061-4236-BA81-DB5184AE77EF}">
+  <dimension ref="A1:I61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>312</v>
+      </c>
+      <c r="I2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>317</v>
+      </c>
+      <c r="I3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>205</v>
+      </c>
+      <c r="I13" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>329</v>
+      </c>
+      <c r="I15" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>340</v>
+      </c>
+      <c r="I17" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>317</v>
+      </c>
+      <c r="I20" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>256</v>
+      </c>
+      <c r="I25" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="I27" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>205</v>
+      </c>
+      <c r="I28" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>332</v>
+      </c>
+      <c r="I30" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>329</v>
+      </c>
+      <c r="I32" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>335</v>
+      </c>
+      <c r="I34" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>317</v>
+      </c>
+      <c r="I35" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="I36" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="I37" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="I38" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>71</v>
+      </c>
+      <c r="I39" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>38</v>
+      </c>
+      <c r="I41" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>205</v>
+      </c>
+      <c r="I42" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>329</v>
+      </c>
+      <c r="I44" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>336</v>
+      </c>
+      <c r="I47" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>317</v>
+      </c>
+      <c r="I48" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="I49" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="I50" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+      <c r="I51" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>71</v>
+      </c>
+      <c r="I54" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>38</v>
+      </c>
+      <c r="I56" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>205</v>
+      </c>
+      <c r="I57" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>329</v>
+      </c>
+      <c r="I59" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>340</v>
+      </c>
+      <c r="I61" t="s">
+        <v>322</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5D5D53-05A0-5640-84B2-9C239538D1C8}">
+  <dimension ref="A1:I35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>428</v>
+      </c>
+      <c r="I1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>208</v>
+      </c>
+      <c r="I5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>205</v>
+      </c>
+      <c r="I8" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>429</v>
+      </c>
+      <c r="I10" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>208</v>
+      </c>
+      <c r="I13" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>208</v>
+      </c>
+      <c r="I17" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>433</v>
+      </c>
+      <c r="I19" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>208</v>
+      </c>
+      <c r="I23" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="I25" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>205</v>
+      </c>
+      <c r="I26" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>434</v>
+      </c>
+      <c r="I28" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="I31" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>208</v>
+      </c>
+      <c r="I32" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="I34" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>205</v>
+      </c>
+      <c r="I35" t="s">
+        <v>420</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{413D21C5-4245-8D43-825A-484E367634AF}">
   <dimension ref="A1:I136"/>
   <sheetViews>
@@ -2738,7 +3510,7 @@
         <v>252</v>
       </c>
       <c r="I134" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
@@ -3771,11 +4543,281 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA227AF4-B786-4A43-BF26-B73CB6A89F8E}">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>435</v>
+      </c>
+      <c r="I2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>208</v>
+      </c>
+      <c r="I15" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>208</v>
+      </c>
+      <c r="I17" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>208</v>
+      </c>
+      <c r="I19" t="s">
+        <v>445</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC48F357-CC96-9947-84F0-7342F43D8D61}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>450</v>
+      </c>
+      <c r="I2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>208</v>
+      </c>
+      <c r="I6" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>451</v>
+      </c>
+      <c r="I7" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>453</v>
+      </c>
+      <c r="I9" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>208</v>
+      </c>
+      <c r="I13" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>205</v>
+      </c>
+      <c r="I16" t="s">
+        <v>420</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC911B4F-D622-4510-AED3-F929CDFD629E}">
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="A13" sqref="A13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3972,10 +5014,10 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>374</v>
+      </c>
+      <c r="I29" t="s">
         <v>375</v>
-      </c>
-      <c r="I29" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -3983,7 +5025,7 @@
         <v>3</v>
       </c>
       <c r="I30" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -3991,7 +5033,7 @@
         <v>4</v>
       </c>
       <c r="I31" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -3999,7 +5041,7 @@
         <v>208</v>
       </c>
       <c r="I32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -4007,7 +5049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E476CB0-A8EA-4A31-AA70-C123E9CDA8B1}">
   <dimension ref="A1:J40"/>
   <sheetViews>
@@ -4279,7 +5321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55DC7D6-6BED-4369-AE88-382318D95376}">
   <dimension ref="A1:I77"/>
   <sheetViews>
@@ -4302,7 +5344,7 @@
         <v>261</v>
       </c>
       <c r="I2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -4310,7 +5352,7 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -4318,7 +5360,7 @@
         <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -4326,7 +5368,7 @@
         <v>204</v>
       </c>
       <c r="I5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -4334,7 +5376,7 @@
         <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -4352,7 +5394,7 @@
         <v>256</v>
       </c>
       <c r="I9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -4370,7 +5412,7 @@
         <v>205</v>
       </c>
       <c r="I12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -4383,7 +5425,7 @@
         <v>231</v>
       </c>
       <c r="I14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -4396,7 +5438,7 @@
         <v>102</v>
       </c>
       <c r="I16" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -4409,10 +5451,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I18" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -4420,15 +5462,15 @@
         <v>329</v>
       </c>
       <c r="I19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>390</v>
+      </c>
+      <c r="I20" t="s">
         <v>391</v>
-      </c>
-      <c r="I20" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -4436,7 +5478,7 @@
         <v>262</v>
       </c>
       <c r="I22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -4444,7 +5486,7 @@
         <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -4452,7 +5494,7 @@
         <v>4</v>
       </c>
       <c r="I24" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -4460,7 +5502,7 @@
         <v>204</v>
       </c>
       <c r="I25" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -4468,7 +5510,7 @@
         <v>6</v>
       </c>
       <c r="I26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -4491,7 +5533,7 @@
         <v>264</v>
       </c>
       <c r="I30" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -4504,7 +5546,7 @@
         <v>256</v>
       </c>
       <c r="I32" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -4562,7 +5604,7 @@
         <v>267</v>
       </c>
       <c r="I44" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -4570,7 +5612,7 @@
         <v>3</v>
       </c>
       <c r="I45" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -4578,7 +5620,7 @@
         <v>4</v>
       </c>
       <c r="I46" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -4586,7 +5628,7 @@
         <v>204</v>
       </c>
       <c r="I47" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -4594,7 +5636,7 @@
         <v>6</v>
       </c>
       <c r="I48" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -4612,12 +5654,12 @@
         <v>264</v>
       </c>
       <c r="I51" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -4640,7 +5682,7 @@
         <v>256</v>
       </c>
       <c r="I56" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -4648,7 +5690,7 @@
         <v>36</v>
       </c>
       <c r="I57" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -4661,12 +5703,12 @@
         <v>205</v>
       </c>
       <c r="I59" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -4674,7 +5716,7 @@
         <v>231</v>
       </c>
       <c r="I61" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
@@ -4687,7 +5729,7 @@
         <v>102</v>
       </c>
       <c r="I63" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
@@ -4700,10 +5742,10 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I65" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -4711,23 +5753,23 @@
         <v>329</v>
       </c>
       <c r="I66" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>390</v>
+      </c>
+      <c r="I67" t="s">
         <v>391</v>
-      </c>
-      <c r="I67" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I68" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -4756,7 +5798,7 @@
         <v>230</v>
       </c>
       <c r="I72" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -4787,7 +5829,7 @@
         <v>208</v>
       </c>
       <c r="I77" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -4795,7 +5837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FD0E9C-3D21-444A-A769-9545E9AA1D4B}">
   <dimension ref="A1:I47"/>
   <sheetViews>
@@ -4818,7 +5860,7 @@
         <v>274</v>
       </c>
       <c r="I2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -4826,7 +5868,7 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -4834,7 +5876,7 @@
         <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -4842,7 +5884,7 @@
         <v>204</v>
       </c>
       <c r="I5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -4850,7 +5892,7 @@
         <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -4863,7 +5905,7 @@
         <v>38</v>
       </c>
       <c r="I8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -4871,23 +5913,23 @@
         <v>205</v>
       </c>
       <c r="I9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="I10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I12" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -4895,7 +5937,7 @@
         <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -4903,7 +5945,7 @@
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -4911,7 +5953,7 @@
         <v>270</v>
       </c>
       <c r="I15" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -4919,7 +5961,7 @@
         <v>6</v>
       </c>
       <c r="I16" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -4927,7 +5969,7 @@
         <v>208</v>
       </c>
       <c r="I17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -4935,7 +5977,7 @@
         <v>271</v>
       </c>
       <c r="I18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -4943,7 +5985,7 @@
         <v>263</v>
       </c>
       <c r="I19" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -4951,7 +5993,7 @@
         <v>264</v>
       </c>
       <c r="I20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -4964,7 +6006,7 @@
         <v>38</v>
       </c>
       <c r="I22" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -4972,7 +6014,7 @@
         <v>205</v>
       </c>
       <c r="I23" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -4985,7 +6027,7 @@
         <v>273</v>
       </c>
       <c r="I25" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -4993,15 +6035,15 @@
         <v>208</v>
       </c>
       <c r="I26" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="I28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -5009,7 +6051,7 @@
         <v>3</v>
       </c>
       <c r="I29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -5017,7 +6059,7 @@
         <v>4</v>
       </c>
       <c r="I30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -5025,7 +6067,7 @@
         <v>6</v>
       </c>
       <c r="I31" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -5038,7 +6080,7 @@
         <v>38</v>
       </c>
       <c r="I33" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -5046,23 +6088,23 @@
         <v>205</v>
       </c>
       <c r="I34" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>424</v>
+      </c>
+      <c r="I35" t="s">
         <v>425</v>
-      </c>
-      <c r="I35" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I37" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -5070,7 +6112,7 @@
         <v>3</v>
       </c>
       <c r="I38" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -5078,7 +6120,7 @@
         <v>4</v>
       </c>
       <c r="I39" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -5086,7 +6128,7 @@
         <v>6</v>
       </c>
       <c r="I40" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -5094,7 +6136,7 @@
         <v>208</v>
       </c>
       <c r="I41" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -5102,7 +6144,7 @@
         <v>271</v>
       </c>
       <c r="I42" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -5110,7 +6152,7 @@
         <v>263</v>
       </c>
       <c r="I43" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -5118,7 +6160,7 @@
         <v>264</v>
       </c>
       <c r="I44" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -5131,7 +6173,7 @@
         <v>38</v>
       </c>
       <c r="I46" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -5139,685 +6181,7 @@
         <v>205</v>
       </c>
       <c r="I47" t="s">
-        <v>421</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E45DC903-E061-4236-BA81-DB5184AE77EF}">
-  <dimension ref="A1:I61"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>312</v>
-      </c>
-      <c r="I2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>317</v>
-      </c>
-      <c r="I3" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>71</v>
-      </c>
-      <c r="I10" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>205</v>
-      </c>
-      <c r="I13" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>329</v>
-      </c>
-      <c r="I15" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>340</v>
-      </c>
-      <c r="I17" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>317</v>
-      </c>
-      <c r="I20" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I21" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="I22" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="I23" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>256</v>
-      </c>
-      <c r="I25" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>38</v>
-      </c>
-      <c r="I27" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>205</v>
-      </c>
-      <c r="I28" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>332</v>
-      </c>
-      <c r="I30" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>329</v>
-      </c>
-      <c r="I32" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>335</v>
-      </c>
-      <c r="I34" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>317</v>
-      </c>
-      <c r="I35" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>3</v>
-      </c>
-      <c r="I36" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="I37" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>6</v>
-      </c>
-      <c r="I38" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>71</v>
-      </c>
-      <c r="I39" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="I41" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>205</v>
-      </c>
-      <c r="I42" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>329</v>
-      </c>
-      <c r="I44" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>336</v>
-      </c>
-      <c r="I47" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>317</v>
-      </c>
-      <c r="I48" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>3</v>
-      </c>
-      <c r="I49" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>4</v>
-      </c>
-      <c r="I50" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>6</v>
-      </c>
-      <c r="I51" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>71</v>
-      </c>
-      <c r="I54" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
-        <v>38</v>
-      </c>
-      <c r="I56" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>205</v>
-      </c>
-      <c r="I57" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>329</v>
-      </c>
-      <c r="I59" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>340</v>
-      </c>
-      <c r="I61" t="s">
-        <v>322</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5D5D53-05A0-5640-84B2-9C239538D1C8}">
-  <dimension ref="A1:I35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>429</v>
-      </c>
-      <c r="I1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>208</v>
-      </c>
-      <c r="I5" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" t="s">
         <v>420</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>205</v>
-      </c>
-      <c r="I8" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>430</v>
-      </c>
-      <c r="I10" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>208</v>
-      </c>
-      <c r="I13" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>96</v>
-      </c>
-      <c r="I15" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>208</v>
-      </c>
-      <c r="I17" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>434</v>
-      </c>
-      <c r="I19" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="I20" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="I21" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="I22" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>208</v>
-      </c>
-      <c r="I23" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>38</v>
-      </c>
-      <c r="I25" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>205</v>
-      </c>
-      <c r="I26" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>435</v>
-      </c>
-      <c r="I28" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="I29" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="I30" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>6</v>
-      </c>
-      <c r="I31" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>208</v>
-      </c>
-      <c r="I32" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>38</v>
-      </c>
-      <c r="I34" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>205</v>
-      </c>
-      <c r="I35" t="s">
-        <v>421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a mapping report.
</commit_message>
<xml_diff>
--- a/CDA-to-FHIR_mappings.xlsx
+++ b/CDA-to-FHIR_mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeanduteau/Dropbox (DDI Work)/HL7 CCDA FHIR Mapping/git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383B1E52-A7FD-7B4E-92EA-282A2F5385B2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD7B2A2-56C5-A847-9864-2D84F89ECA6E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19000" xr2:uid="{BECB9657-49B2-1141-A8A5-81EA227BF036}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1939" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="732">
   <si>
     <t>realmCode</t>
   </si>
@@ -7830,8 +7830,8 @@
   </sheetPr>
   <dimension ref="A1:K143"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="I135" sqref="I135"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7896,9 +7896,6 @@
         <v>40</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="I7" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
@@ -7966,9 +7963,6 @@
         <v>40</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="I16" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
@@ -8035,9 +8029,6 @@
         <v>41</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="I25" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
@@ -8270,9 +8261,6 @@
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>16</v>
-      </c>
-      <c r="I55" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>